<commit_message>
Aplicado cambios menores para depuracion
</commit_message>
<xml_diff>
--- a/gral-escobedo.xlsx
+++ b/gral-escobedo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\airq-scrapper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\airq-scrapper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2ED8B79-78E2-47B2-A9F9-2FF389D01ED7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B115ADB9-5BC1-4405-AB8F-77B991B79729}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{13C4C640-B4B7-4E62-8E49-78859A122DF2}"/>
+    <workbookView xWindow="3480" yWindow="2490" windowWidth="22530" windowHeight="18390" xr2:uid="{13C4C640-B4B7-4E62-8E49-78859A122DF2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Fecha</t>
   </si>
   <si>
-    <t>PM2.5</t>
-  </si>
-  <si>
     <t>PM10</t>
   </si>
   <si>
@@ -57,6 +54,9 @@
   </si>
   <si>
     <t>CO</t>
+  </si>
+  <si>
+    <t>PM2,5</t>
   </si>
 </sst>
 </file>
@@ -263,7 +263,7 @@
   <autoFilter ref="A1:G86" xr:uid="{501EB3A9-2C7B-43C9-BCA7-538D5EDACF8C}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{5B4B24C3-FC4B-444E-8861-6B959A254DC6}" name="Fecha" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{888BCB63-18BD-4AA4-8B1D-130BD34B6428}" name="PM2.5" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{888BCB63-18BD-4AA4-8B1D-130BD34B6428}" name="PM2,5" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{A7BA20F9-8CD0-4F17-A827-B9F96E10394C}" name="PM10" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{20600A59-399C-40D3-BA9A-ADF54BF11781}" name="O3" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{820A6234-B7A5-4C29-8B10-D9FC2ADDD617}" name="NO2" dataDxfId="2"/>
@@ -275,7 +275,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -593,11 +593,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA81F182-727E-4309-A6F6-61F530C30CCD}">
   <dimension ref="A1:G86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="N87" sqref="N87"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
@@ -613,22 +613,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="21" x14ac:dyDescent="0.35">

</xml_diff>